<commit_message>
Adding merge tables to Working with Excel files
</commit_message>
<xml_diff>
--- a/lectures/working_with_excel_files/output/merged_table.xlsx
+++ b/lectures/working_with_excel_files/output/merged_table.xlsx
@@ -15,7 +15,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="146">
   <si>
-    <t>ID_inv_data</t>
+    <t>ID_inventory_table</t>
   </si>
   <si>
     <t>Mouse_1</t>
@@ -321,7 +321,7 @@
     <t>Used</t>
   </si>
   <si>
-    <t>ID_pheno_data</t>
+    <t>ID_phenotype_table</t>
   </si>
   <si>
     <t>Mouse_1</t>
@@ -499,12 +499,12 @@
   <dimension ref="A1:J55"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.578125" customWidth="true"/>
+    <col min="1" max="1" width="16.1796875" customWidth="true"/>
     <col min="2" max="2" width="4.11328125" customWidth="true"/>
     <col min="3" max="3" width="11.3125" customWidth="true"/>
     <col min="4" max="4" width="10.3125" customWidth="true"/>
     <col min="5" max="5" width="8.37890625" customWidth="true"/>
-    <col min="6" max="6" width="13.1796875" customWidth="true"/>
+    <col min="6" max="6" width="17.11328125" customWidth="true"/>
     <col min="7" max="7" width="6.84375" customWidth="true"/>
     <col min="8" max="8" width="8.77734375" customWidth="true"/>
     <col min="9" max="9" width="11.64453125" customWidth="true"/>

</xml_diff>